<commit_message>
Try inserting value into cell :bear:
</commit_message>
<xml_diff>
--- a/python/openpyxl/financial_sample.xlsx
+++ b/python/openpyxl/financial_sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7770" windowWidth="23595" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7770" windowWidth="23595" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Finances 2017" sheetId="1" state="visible" r:id="rId1"/>
@@ -35823,7 +35823,7 @@
     </row>
     <row r="703" spans="1:16">
       <c r="L703">
-        <f>SUM(L2:L702)</f>
+        <f>SUM(L2:L10)</f>
         <v/>
       </c>
       <c r="M703">

</xml_diff>